<commit_message>
Update urenverantwoording sjabloom Jesse Ernste.xlsx
</commit_message>
<xml_diff>
--- a/Documentatie/Urenverantwoording/Jesse/urenverantwoording sjabloom Jesse Ernste.xlsx
+++ b/Documentatie/Urenverantwoording/Jesse/urenverantwoording sjabloom Jesse Ernste.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesse\Documents\GitHub\Project-digitale-besturing\Documentatie\Notules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesse\Documents\GitHub\Project-digitale-besturing\Documentatie\Urenverantwoording\Jesse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB0ADFC-E51A-48ED-BA06-6D9DB590AD02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1872969-B249-45FD-A517-2A278ECA7889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -795,6 +795,18 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="5" fillId="5" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="5" fillId="6" borderId="37" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="6" borderId="5" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -859,18 +871,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="6" borderId="37" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="6" borderId="5" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1176,7 +1176,7 @@
                   <c:v>0.14583333333333337</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.2499999999999944E-2</c:v>
+                  <c:v>0.10416666666666663</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1400,7 +1400,7 @@
                   <c:v>0.14583333333333337</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.2499999999999944E-2</c:v>
+                  <c:v>0.10416666666666663</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1765,7 +1765,7 @@
                   <c:v>0.14583333333333337</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.2499999999999944E-2</c:v>
+                  <c:v>0.10416666666666663</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2132,7 +2132,7 @@
                   <c:v>0.14583333333333337</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.2499999999999944E-2</c:v>
+                  <c:v>0.10416666666666663</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2808,7 +2808,7 @@
                 <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.20833333333333331</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -3195,7 +3195,7 @@
                   <c:v>0.14583333333333337</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.2499999999999944E-2</c:v>
+                  <c:v>0.10416666666666663</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -6993,7 +6993,7 @@
                   <c:v>0.14583333333333337</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.2499999999999944E-2</c:v>
+                  <c:v>0.10416666666666663</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -14057,8 +14057,8 @@
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:N18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14138,10 +14138,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="72" t="s">
+      <c r="C4" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="72"/>
+      <c r="D4" s="52"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -14149,10 +14149,10 @@
         <v>6</v>
       </c>
       <c r="I4" s="2"/>
-      <c r="J4" s="72" t="s">
+      <c r="J4" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="K4" s="72"/>
+      <c r="K4" s="52"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -14178,10 +14178,10 @@
         <v>7</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="72" t="s">
+      <c r="C6" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="72"/>
+      <c r="D6" s="52"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -14189,10 +14189,10 @@
         <v>8</v>
       </c>
       <c r="I6" s="2"/>
-      <c r="J6" s="72" t="s">
+      <c r="J6" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="K6" s="72"/>
+      <c r="K6" s="52"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -14259,19 +14259,19 @@
       <c r="C10" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="73" t="s">
+      <c r="D10" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="73"/>
-      <c r="N10" s="73"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="53"/>
+      <c r="M10" s="53"/>
+      <c r="N10" s="53"/>
       <c r="O10" s="43" t="s">
         <v>38</v>
       </c>
@@ -14280,25 +14280,25 @@
       <c r="A11" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="50">
+      <c r="B11" s="54">
         <f>C12-C11-O11</f>
         <v>0</v>
       </c>
       <c r="C11" s="27">
         <v>0</v>
       </c>
-      <c r="D11" s="52"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="53"/>
-      <c r="N11" s="54"/>
-      <c r="O11" s="74">
+      <c r="D11" s="56"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="50">
         <v>0</v>
       </c>
       <c r="P11" s="35"/>
@@ -14309,22 +14309,22 @@
         <f>F2</f>
         <v>45693</v>
       </c>
-      <c r="B12" s="51"/>
+      <c r="B12" s="55"/>
       <c r="C12" s="26">
         <v>0</v>
       </c>
-      <c r="D12" s="55"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="56"/>
-      <c r="L12" s="56"/>
-      <c r="M12" s="56"/>
-      <c r="N12" s="57"/>
-      <c r="O12" s="75"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="60"/>
+      <c r="N12" s="61"/>
+      <c r="O12" s="51"/>
       <c r="P12" s="35"/>
       <c r="Q12" s="18"/>
     </row>
@@ -14332,25 +14332,25 @@
       <c r="A13" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="71">
+      <c r="B13" s="75">
         <f>C14-C13-O13</f>
         <v>0</v>
       </c>
       <c r="C13" s="27">
         <v>0</v>
       </c>
-      <c r="D13" s="58"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59"/>
-      <c r="N13" s="60"/>
-      <c r="O13" s="74">
+      <c r="D13" s="62"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="63"/>
+      <c r="L13" s="63"/>
+      <c r="M13" s="63"/>
+      <c r="N13" s="64"/>
+      <c r="O13" s="50">
         <v>0</v>
       </c>
       <c r="P13" s="35"/>
@@ -14361,22 +14361,22 @@
         <f>A12+1</f>
         <v>45694</v>
       </c>
-      <c r="B14" s="51"/>
+      <c r="B14" s="55"/>
       <c r="C14" s="26">
         <v>0</v>
       </c>
-      <c r="D14" s="55"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="56"/>
-      <c r="L14" s="56"/>
-      <c r="M14" s="56"/>
-      <c r="N14" s="57"/>
-      <c r="O14" s="75"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="60"/>
+      <c r="N14" s="61"/>
+      <c r="O14" s="51"/>
       <c r="P14" s="35"/>
       <c r="Q14" s="18"/>
     </row>
@@ -14384,27 +14384,27 @@
       <c r="A15" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="71">
+      <c r="B15" s="75">
         <f>C16-C15-O15</f>
         <v>0.14583333333333337</v>
       </c>
       <c r="C15" s="27">
         <v>0.4375</v>
       </c>
-      <c r="D15" s="58" t="s">
+      <c r="D15" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="59"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="59"/>
-      <c r="N15" s="60"/>
-      <c r="O15" s="74">
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="63"/>
+      <c r="L15" s="63"/>
+      <c r="M15" s="63"/>
+      <c r="N15" s="64"/>
+      <c r="O15" s="50">
         <v>0</v>
       </c>
       <c r="P15" s="35"/>
@@ -14415,48 +14415,48 @@
         <f>A14+1</f>
         <v>45695</v>
       </c>
-      <c r="B16" s="51"/>
+      <c r="B16" s="55"/>
       <c r="C16" s="26">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D16" s="55"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="56"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="56"/>
-      <c r="L16" s="56"/>
-      <c r="M16" s="56"/>
-      <c r="N16" s="57"/>
-      <c r="O16" s="75"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="60"/>
+      <c r="L16" s="60"/>
+      <c r="M16" s="60"/>
+      <c r="N16" s="61"/>
+      <c r="O16" s="51"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="71">
+      <c r="B17" s="75">
         <f>C18-C17-O17</f>
-        <v>6.2499999999999944E-2</v>
+        <v>0.10416666666666663</v>
       </c>
       <c r="C17" s="27">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="D17" s="58" t="s">
+        <v>0.4375</v>
+      </c>
+      <c r="D17" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="59"/>
-      <c r="H17" s="59"/>
-      <c r="I17" s="59"/>
-      <c r="J17" s="59"/>
-      <c r="K17" s="59"/>
-      <c r="L17" s="59"/>
-      <c r="M17" s="59"/>
-      <c r="N17" s="60"/>
-      <c r="O17" s="74">
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="63"/>
+      <c r="L17" s="63"/>
+      <c r="M17" s="63"/>
+      <c r="N17" s="64"/>
+      <c r="O17" s="50">
         <v>0</v>
       </c>
     </row>
@@ -14465,46 +14465,46 @@
         <f>A16+1</f>
         <v>45696</v>
       </c>
-      <c r="B18" s="51"/>
+      <c r="B18" s="55"/>
       <c r="C18" s="26">
         <v>0.54166666666666663</v>
       </c>
-      <c r="D18" s="55"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="56"/>
-      <c r="K18" s="56"/>
-      <c r="L18" s="56"/>
-      <c r="M18" s="56"/>
-      <c r="N18" s="57"/>
-      <c r="O18" s="75"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="60"/>
+      <c r="N18" s="61"/>
+      <c r="O18" s="51"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="71">
+      <c r="B19" s="75">
         <f>C20-C19-O19</f>
         <v>0</v>
       </c>
       <c r="C19" s="27">
         <v>0</v>
       </c>
-      <c r="D19" s="58"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="59"/>
-      <c r="H19" s="59"/>
-      <c r="I19" s="59"/>
-      <c r="J19" s="59"/>
-      <c r="K19" s="59"/>
-      <c r="L19" s="59"/>
-      <c r="M19" s="59"/>
-      <c r="N19" s="60"/>
-      <c r="O19" s="74">
+      <c r="D19" s="62"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="63"/>
+      <c r="L19" s="63"/>
+      <c r="M19" s="63"/>
+      <c r="N19" s="64"/>
+      <c r="O19" s="50">
         <v>0</v>
       </c>
     </row>
@@ -14513,22 +14513,22 @@
         <f>A18+1</f>
         <v>45697</v>
       </c>
-      <c r="B20" s="51"/>
+      <c r="B20" s="55"/>
       <c r="C20" s="26">
         <v>0</v>
       </c>
-      <c r="D20" s="55"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="56"/>
-      <c r="K20" s="56"/>
-      <c r="L20" s="56"/>
-      <c r="M20" s="56"/>
-      <c r="N20" s="57"/>
-      <c r="O20" s="75"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="60"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="60"/>
+      <c r="J20" s="60"/>
+      <c r="K20" s="60"/>
+      <c r="L20" s="60"/>
+      <c r="M20" s="60"/>
+      <c r="N20" s="61"/>
+      <c r="O20" s="51"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
@@ -14547,7 +14547,7 @@
       <c r="N21" s="2"/>
     </row>
     <row r="22" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="61" t="s">
+      <c r="A22" s="65" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="14" t="s">
@@ -14569,51 +14569,51 @@
       <c r="N22" s="2"/>
     </row>
     <row r="23" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="62"/>
-      <c r="B23" s="64"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="64"/>
-      <c r="I23" s="65"/>
-      <c r="J23" s="65"/>
-      <c r="K23" s="65"/>
-      <c r="L23" s="65"/>
-      <c r="M23" s="66"/>
+      <c r="A23" s="66"/>
+      <c r="B23" s="68"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="69"/>
+      <c r="J23" s="69"/>
+      <c r="K23" s="69"/>
+      <c r="L23" s="69"/>
+      <c r="M23" s="70"/>
       <c r="N23" s="2"/>
     </row>
     <row r="24" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="62"/>
-      <c r="B24" s="67"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="67"/>
-      <c r="I24" s="65"/>
-      <c r="J24" s="65"/>
-      <c r="K24" s="65"/>
-      <c r="L24" s="65"/>
-      <c r="M24" s="66"/>
+      <c r="A24" s="66"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="69"/>
+      <c r="K24" s="69"/>
+      <c r="L24" s="69"/>
+      <c r="M24" s="70"/>
       <c r="N24" s="2"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="63"/>
-      <c r="B25" s="68"/>
-      <c r="C25" s="69"/>
-      <c r="D25" s="69"/>
-      <c r="E25" s="69"/>
-      <c r="F25" s="69"/>
-      <c r="G25" s="70"/>
-      <c r="H25" s="68"/>
-      <c r="I25" s="69"/>
-      <c r="J25" s="69"/>
-      <c r="K25" s="69"/>
-      <c r="L25" s="69"/>
-      <c r="M25" s="70"/>
+      <c r="A25" s="67"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="73"/>
+      <c r="J25" s="73"/>
+      <c r="K25" s="73"/>
+      <c r="L25" s="73"/>
+      <c r="M25" s="74"/>
       <c r="N25" s="2"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
@@ -14640,7 +14640,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="49">
         <f>B11+B13+B15+B17+B19</f>
-        <v>0.20833333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
@@ -14663,7 +14663,7 @@
       <c r="C28" s="2"/>
       <c r="D28" s="49">
         <f>SUM(B11:B20)</f>
-        <v>0.20833333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2" t="s">
@@ -14683,16 +14683,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="O17:O18"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="D10:N10"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="D11:N12"/>
     <mergeCell ref="D13:N14"/>
@@ -14706,6 +14696,16 @@
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="D17:N18"/>
     <mergeCell ref="D19:N20"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="D10:N10"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="O17:O18"/>
+    <mergeCell ref="O19:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -14995,11 +14995,11 @@
         <v>5</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="72" t="str">
+      <c r="C4" s="52" t="str">
         <f>'week 1'!C4</f>
         <v>Jesse</v>
       </c>
-      <c r="D4" s="72"/>
+      <c r="D4" s="52"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -15007,11 +15007,11 @@
         <v>6</v>
       </c>
       <c r="I4" s="2"/>
-      <c r="J4" s="72" t="str">
+      <c r="J4" s="52" t="str">
         <f>'week 1'!J4</f>
         <v>NHL Stenden</v>
       </c>
-      <c r="K4" s="72"/>
+      <c r="K4" s="52"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -15037,11 +15037,11 @@
         <v>7</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="72" t="str">
+      <c r="C6" s="52" t="str">
         <f>'week 1'!C6</f>
         <v>Hendrik Bijlsma</v>
       </c>
-      <c r="D6" s="72"/>
+      <c r="D6" s="52"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -15049,11 +15049,11 @@
         <v>8</v>
       </c>
       <c r="I6" s="2"/>
-      <c r="J6" s="72" t="str">
+      <c r="J6" s="52" t="str">
         <f>'week 1'!J6</f>
         <v>Cees Naatvlees</v>
       </c>
-      <c r="K6" s="72"/>
+      <c r="K6" s="52"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -15120,18 +15120,18 @@
       <c r="C10" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="73" t="s">
+      <c r="D10" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="73"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="53"/>
+      <c r="M10" s="53"/>
       <c r="N10" s="76"/>
       <c r="O10" s="43" t="s">
         <v>38</v>
@@ -15141,25 +15141,25 @@
       <c r="A11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="71">
+      <c r="B11" s="75">
         <f>C12-C11-O11</f>
         <v>0</v>
       </c>
       <c r="C11" s="27">
         <v>0</v>
       </c>
-      <c r="D11" s="52"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="53"/>
-      <c r="N11" s="54"/>
-      <c r="O11" s="74">
+      <c r="D11" s="56"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="50">
         <v>0</v>
       </c>
     </row>
@@ -15168,46 +15168,46 @@
         <f>F2</f>
         <v>45700</v>
       </c>
-      <c r="B12" s="51"/>
+      <c r="B12" s="55"/>
       <c r="C12" s="26">
         <v>0</v>
       </c>
-      <c r="D12" s="55"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="56"/>
-      <c r="L12" s="56"/>
-      <c r="M12" s="56"/>
-      <c r="N12" s="57"/>
-      <c r="O12" s="75"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="60"/>
+      <c r="N12" s="61"/>
+      <c r="O12" s="51"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="71">
+      <c r="B13" s="75">
         <f>C14-C13-O13</f>
         <v>0</v>
       </c>
       <c r="C13" s="27">
         <v>0</v>
       </c>
-      <c r="D13" s="58"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59"/>
-      <c r="N13" s="60"/>
-      <c r="O13" s="74">
+      <c r="D13" s="62"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="63"/>
+      <c r="L13" s="63"/>
+      <c r="M13" s="63"/>
+      <c r="N13" s="64"/>
+      <c r="O13" s="50">
         <v>0</v>
       </c>
     </row>
@@ -15216,46 +15216,46 @@
         <f>A12+1</f>
         <v>45701</v>
       </c>
-      <c r="B14" s="51"/>
+      <c r="B14" s="55"/>
       <c r="C14" s="26">
         <v>0</v>
       </c>
-      <c r="D14" s="55"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="56"/>
-      <c r="L14" s="56"/>
-      <c r="M14" s="56"/>
-      <c r="N14" s="57"/>
-      <c r="O14" s="75"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="60"/>
+      <c r="N14" s="61"/>
+      <c r="O14" s="51"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="71">
+      <c r="B15" s="75">
         <f>C16-C15-O15</f>
         <v>0</v>
       </c>
       <c r="C15" s="27">
         <v>0</v>
       </c>
-      <c r="D15" s="58"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="59"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="59"/>
-      <c r="N15" s="60"/>
-      <c r="O15" s="74">
+      <c r="D15" s="62"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="63"/>
+      <c r="L15" s="63"/>
+      <c r="M15" s="63"/>
+      <c r="N15" s="64"/>
+      <c r="O15" s="50">
         <v>0</v>
       </c>
     </row>
@@ -15264,46 +15264,46 @@
         <f>A14+1</f>
         <v>45702</v>
       </c>
-      <c r="B16" s="51"/>
+      <c r="B16" s="55"/>
       <c r="C16" s="26">
         <v>0</v>
       </c>
-      <c r="D16" s="55"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="56"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="56"/>
-      <c r="L16" s="56"/>
-      <c r="M16" s="56"/>
-      <c r="N16" s="57"/>
-      <c r="O16" s="75"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="60"/>
+      <c r="L16" s="60"/>
+      <c r="M16" s="60"/>
+      <c r="N16" s="61"/>
+      <c r="O16" s="51"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="71">
+      <c r="B17" s="75">
         <f>C18-C17-O17</f>
         <v>0</v>
       </c>
       <c r="C17" s="27">
         <v>0</v>
       </c>
-      <c r="D17" s="58"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="59"/>
-      <c r="H17" s="59"/>
-      <c r="I17" s="59"/>
-      <c r="J17" s="59"/>
-      <c r="K17" s="59"/>
-      <c r="L17" s="59"/>
-      <c r="M17" s="59"/>
-      <c r="N17" s="60"/>
-      <c r="O17" s="74">
+      <c r="D17" s="62"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="63"/>
+      <c r="L17" s="63"/>
+      <c r="M17" s="63"/>
+      <c r="N17" s="64"/>
+      <c r="O17" s="50">
         <v>0</v>
       </c>
     </row>
@@ -15312,46 +15312,46 @@
         <f>A16+1</f>
         <v>45703</v>
       </c>
-      <c r="B18" s="51"/>
+      <c r="B18" s="55"/>
       <c r="C18" s="26">
         <v>0</v>
       </c>
-      <c r="D18" s="55"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="56"/>
-      <c r="K18" s="56"/>
-      <c r="L18" s="56"/>
-      <c r="M18" s="56"/>
-      <c r="N18" s="57"/>
-      <c r="O18" s="75"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="60"/>
+      <c r="N18" s="61"/>
+      <c r="O18" s="51"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="71">
+      <c r="B19" s="75">
         <f>C20-C19-O19</f>
         <v>0</v>
       </c>
       <c r="C19" s="27">
         <v>0</v>
       </c>
-      <c r="D19" s="58"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="59"/>
-      <c r="H19" s="59"/>
-      <c r="I19" s="59"/>
-      <c r="J19" s="59"/>
-      <c r="K19" s="59"/>
-      <c r="L19" s="59"/>
-      <c r="M19" s="59"/>
-      <c r="N19" s="60"/>
-      <c r="O19" s="74">
+      <c r="D19" s="62"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="63"/>
+      <c r="L19" s="63"/>
+      <c r="M19" s="63"/>
+      <c r="N19" s="64"/>
+      <c r="O19" s="50">
         <v>0</v>
       </c>
     </row>
@@ -15360,22 +15360,22 @@
         <f>A18+1</f>
         <v>45704</v>
       </c>
-      <c r="B20" s="51"/>
+      <c r="B20" s="55"/>
       <c r="C20" s="26">
         <v>0</v>
       </c>
-      <c r="D20" s="55"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="56"/>
-      <c r="K20" s="56"/>
-      <c r="L20" s="56"/>
-      <c r="M20" s="56"/>
-      <c r="N20" s="57"/>
-      <c r="O20" s="75"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="60"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="60"/>
+      <c r="J20" s="60"/>
+      <c r="K20" s="60"/>
+      <c r="L20" s="60"/>
+      <c r="M20" s="60"/>
+      <c r="N20" s="61"/>
+      <c r="O20" s="51"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
@@ -15394,7 +15394,7 @@
       <c r="N21" s="2"/>
     </row>
     <row r="22" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="61" t="s">
+      <c r="A22" s="65" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="14" t="s">
@@ -15416,51 +15416,51 @@
       <c r="N22" s="2"/>
     </row>
     <row r="23" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="62"/>
-      <c r="B23" s="64"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="64"/>
-      <c r="I23" s="65"/>
-      <c r="J23" s="65"/>
-      <c r="K23" s="65"/>
-      <c r="L23" s="65"/>
-      <c r="M23" s="66"/>
+      <c r="A23" s="66"/>
+      <c r="B23" s="68"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="69"/>
+      <c r="J23" s="69"/>
+      <c r="K23" s="69"/>
+      <c r="L23" s="69"/>
+      <c r="M23" s="70"/>
       <c r="N23" s="2"/>
     </row>
     <row r="24" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="62"/>
-      <c r="B24" s="67"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="67"/>
-      <c r="I24" s="65"/>
-      <c r="J24" s="65"/>
-      <c r="K24" s="65"/>
-      <c r="L24" s="65"/>
-      <c r="M24" s="66"/>
+      <c r="A24" s="66"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="69"/>
+      <c r="K24" s="69"/>
+      <c r="L24" s="69"/>
+      <c r="M24" s="70"/>
       <c r="N24" s="2"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="63"/>
-      <c r="B25" s="68"/>
-      <c r="C25" s="69"/>
-      <c r="D25" s="69"/>
-      <c r="E25" s="69"/>
-      <c r="F25" s="69"/>
-      <c r="G25" s="70"/>
-      <c r="H25" s="68"/>
-      <c r="I25" s="69"/>
-      <c r="J25" s="69"/>
-      <c r="K25" s="69"/>
-      <c r="L25" s="69"/>
-      <c r="M25" s="70"/>
+      <c r="A25" s="67"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="73"/>
+      <c r="J25" s="73"/>
+      <c r="K25" s="73"/>
+      <c r="L25" s="73"/>
+      <c r="M25" s="74"/>
       <c r="N25" s="2"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
@@ -15487,7 +15487,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="49">
         <f>SUM(B11:B20,'week 1'!D27)</f>
-        <v>0.20833333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
@@ -15533,11 +15533,15 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="O17:O18"/>
-    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="D10:N10"/>
+    <mergeCell ref="D11:N12"/>
+    <mergeCell ref="D13:N14"/>
     <mergeCell ref="D15:N16"/>
     <mergeCell ref="D17:N18"/>
     <mergeCell ref="D19:N20"/>
@@ -15547,15 +15551,11 @@
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="B19:B20"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="D10:N10"/>
-    <mergeCell ref="D11:N12"/>
-    <mergeCell ref="D13:N14"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="O17:O18"/>
+    <mergeCell ref="O19:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15647,11 +15647,11 @@
         <v>5</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="72" t="str">
+      <c r="C4" s="52" t="str">
         <f>'week 1'!C4</f>
         <v>Jesse</v>
       </c>
-      <c r="D4" s="72"/>
+      <c r="D4" s="52"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -15659,11 +15659,11 @@
         <v>6</v>
       </c>
       <c r="I4" s="2"/>
-      <c r="J4" s="72" t="str">
+      <c r="J4" s="52" t="str">
         <f>'week 1'!J4</f>
         <v>NHL Stenden</v>
       </c>
-      <c r="K4" s="72"/>
+      <c r="K4" s="52"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -15689,11 +15689,11 @@
         <v>7</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="72" t="str">
+      <c r="C6" s="52" t="str">
         <f>'week 1'!C6</f>
         <v>Hendrik Bijlsma</v>
       </c>
-      <c r="D6" s="72"/>
+      <c r="D6" s="52"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -15701,11 +15701,11 @@
         <v>8</v>
       </c>
       <c r="I6" s="2"/>
-      <c r="J6" s="72" t="str">
+      <c r="J6" s="52" t="str">
         <f>'week 1'!J6</f>
         <v>Cees Naatvlees</v>
       </c>
-      <c r="K6" s="72"/>
+      <c r="K6" s="52"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -15772,18 +15772,18 @@
       <c r="C10" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="73" t="s">
+      <c r="D10" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="73"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="53"/>
+      <c r="M10" s="53"/>
       <c r="N10" s="76"/>
       <c r="O10" s="43" t="s">
         <v>38</v>
@@ -15793,25 +15793,25 @@
       <c r="A11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="71">
+      <c r="B11" s="75">
         <f>C12-C11-O11</f>
         <v>0</v>
       </c>
       <c r="C11" s="27">
         <v>0</v>
       </c>
-      <c r="D11" s="52"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="53"/>
-      <c r="N11" s="54"/>
-      <c r="O11" s="74">
+      <c r="D11" s="56"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="50">
         <v>0</v>
       </c>
     </row>
@@ -15820,46 +15820,46 @@
         <f>F2</f>
         <v>45707</v>
       </c>
-      <c r="B12" s="51"/>
+      <c r="B12" s="55"/>
       <c r="C12" s="26">
         <v>0</v>
       </c>
-      <c r="D12" s="55"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="56"/>
-      <c r="L12" s="56"/>
-      <c r="M12" s="56"/>
-      <c r="N12" s="57"/>
-      <c r="O12" s="75"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="60"/>
+      <c r="N12" s="61"/>
+      <c r="O12" s="51"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="71">
+      <c r="B13" s="75">
         <f>C14-C13-O13</f>
         <v>0</v>
       </c>
       <c r="C13" s="27">
         <v>0</v>
       </c>
-      <c r="D13" s="58"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59"/>
-      <c r="N13" s="60"/>
-      <c r="O13" s="74">
+      <c r="D13" s="62"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="63"/>
+      <c r="L13" s="63"/>
+      <c r="M13" s="63"/>
+      <c r="N13" s="64"/>
+      <c r="O13" s="50">
         <v>0</v>
       </c>
     </row>
@@ -15868,46 +15868,46 @@
         <f>A12+1</f>
         <v>45708</v>
       </c>
-      <c r="B14" s="51"/>
+      <c r="B14" s="55"/>
       <c r="C14" s="26">
         <v>0</v>
       </c>
-      <c r="D14" s="55"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="56"/>
-      <c r="L14" s="56"/>
-      <c r="M14" s="56"/>
-      <c r="N14" s="57"/>
-      <c r="O14" s="75"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="60"/>
+      <c r="N14" s="61"/>
+      <c r="O14" s="51"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="71">
+      <c r="B15" s="75">
         <f>C16-C15-O15</f>
         <v>0</v>
       </c>
       <c r="C15" s="27">
         <v>0</v>
       </c>
-      <c r="D15" s="58"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="59"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="59"/>
-      <c r="N15" s="60"/>
-      <c r="O15" s="74">
+      <c r="D15" s="62"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="63"/>
+      <c r="L15" s="63"/>
+      <c r="M15" s="63"/>
+      <c r="N15" s="64"/>
+      <c r="O15" s="50">
         <v>0</v>
       </c>
     </row>
@@ -15916,46 +15916,46 @@
         <f>A14+1</f>
         <v>45709</v>
       </c>
-      <c r="B16" s="51"/>
+      <c r="B16" s="55"/>
       <c r="C16" s="26">
         <v>0</v>
       </c>
-      <c r="D16" s="55"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="56"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="56"/>
-      <c r="L16" s="56"/>
-      <c r="M16" s="56"/>
-      <c r="N16" s="57"/>
-      <c r="O16" s="75"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="60"/>
+      <c r="L16" s="60"/>
+      <c r="M16" s="60"/>
+      <c r="N16" s="61"/>
+      <c r="O16" s="51"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="71">
+      <c r="B17" s="75">
         <f>C18-C17-O17</f>
         <v>0</v>
       </c>
       <c r="C17" s="27">
         <v>0</v>
       </c>
-      <c r="D17" s="58"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="59"/>
-      <c r="H17" s="59"/>
-      <c r="I17" s="59"/>
-      <c r="J17" s="59"/>
-      <c r="K17" s="59"/>
-      <c r="L17" s="59"/>
-      <c r="M17" s="59"/>
-      <c r="N17" s="60"/>
-      <c r="O17" s="74">
+      <c r="D17" s="62"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="63"/>
+      <c r="L17" s="63"/>
+      <c r="M17" s="63"/>
+      <c r="N17" s="64"/>
+      <c r="O17" s="50">
         <v>0</v>
       </c>
     </row>
@@ -15964,46 +15964,46 @@
         <f>A16+1</f>
         <v>45710</v>
       </c>
-      <c r="B18" s="51"/>
+      <c r="B18" s="55"/>
       <c r="C18" s="26">
         <v>0</v>
       </c>
-      <c r="D18" s="55"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="56"/>
-      <c r="K18" s="56"/>
-      <c r="L18" s="56"/>
-      <c r="M18" s="56"/>
-      <c r="N18" s="57"/>
-      <c r="O18" s="75"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="60"/>
+      <c r="N18" s="61"/>
+      <c r="O18" s="51"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="71">
+      <c r="B19" s="75">
         <f>C20-C19-O19</f>
         <v>0</v>
       </c>
       <c r="C19" s="27">
         <v>0</v>
       </c>
-      <c r="D19" s="58"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="59"/>
-      <c r="H19" s="59"/>
-      <c r="I19" s="59"/>
-      <c r="J19" s="59"/>
-      <c r="K19" s="59"/>
-      <c r="L19" s="59"/>
-      <c r="M19" s="59"/>
-      <c r="N19" s="60"/>
-      <c r="O19" s="74">
+      <c r="D19" s="62"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="63"/>
+      <c r="L19" s="63"/>
+      <c r="M19" s="63"/>
+      <c r="N19" s="64"/>
+      <c r="O19" s="50">
         <v>0</v>
       </c>
     </row>
@@ -16012,22 +16012,22 @@
         <f>A18+1</f>
         <v>45711</v>
       </c>
-      <c r="B20" s="51"/>
+      <c r="B20" s="55"/>
       <c r="C20" s="26">
         <v>0</v>
       </c>
-      <c r="D20" s="55"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="56"/>
-      <c r="K20" s="56"/>
-      <c r="L20" s="56"/>
-      <c r="M20" s="56"/>
-      <c r="N20" s="57"/>
-      <c r="O20" s="75"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="60"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="60"/>
+      <c r="J20" s="60"/>
+      <c r="K20" s="60"/>
+      <c r="L20" s="60"/>
+      <c r="M20" s="60"/>
+      <c r="N20" s="61"/>
+      <c r="O20" s="51"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
@@ -16046,7 +16046,7 @@
       <c r="N21" s="2"/>
     </row>
     <row r="22" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="61" t="s">
+      <c r="A22" s="65" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="14" t="s">
@@ -16068,51 +16068,51 @@
       <c r="N22" s="2"/>
     </row>
     <row r="23" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="62"/>
-      <c r="B23" s="64"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="64"/>
-      <c r="I23" s="65"/>
-      <c r="J23" s="65"/>
-      <c r="K23" s="65"/>
-      <c r="L23" s="65"/>
-      <c r="M23" s="66"/>
+      <c r="A23" s="66"/>
+      <c r="B23" s="68"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="69"/>
+      <c r="J23" s="69"/>
+      <c r="K23" s="69"/>
+      <c r="L23" s="69"/>
+      <c r="M23" s="70"/>
       <c r="N23" s="2"/>
     </row>
     <row r="24" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="62"/>
-      <c r="B24" s="67"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="67"/>
-      <c r="I24" s="65"/>
-      <c r="J24" s="65"/>
-      <c r="K24" s="65"/>
-      <c r="L24" s="65"/>
-      <c r="M24" s="66"/>
+      <c r="A24" s="66"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="69"/>
+      <c r="K24" s="69"/>
+      <c r="L24" s="69"/>
+      <c r="M24" s="70"/>
       <c r="N24" s="2"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="63"/>
-      <c r="B25" s="68"/>
-      <c r="C25" s="69"/>
-      <c r="D25" s="69"/>
-      <c r="E25" s="69"/>
-      <c r="F25" s="69"/>
-      <c r="G25" s="70"/>
-      <c r="H25" s="68"/>
-      <c r="I25" s="69"/>
-      <c r="J25" s="69"/>
-      <c r="K25" s="69"/>
-      <c r="L25" s="69"/>
-      <c r="M25" s="70"/>
+      <c r="A25" s="67"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="73"/>
+      <c r="J25" s="73"/>
+      <c r="K25" s="73"/>
+      <c r="L25" s="73"/>
+      <c r="M25" s="74"/>
       <c r="N25" s="2"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
@@ -16139,7 +16139,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="49">
         <f>SUM(B11:B20,'week 2'!D27)</f>
-        <v>0.20833333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
@@ -16182,16 +16182,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="O17:O18"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="D10:N10"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="D11:N12"/>
     <mergeCell ref="D13:N14"/>
@@ -16205,6 +16195,16 @@
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="D17:N18"/>
     <mergeCell ref="D19:N20"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="D10:N10"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="O17:O18"/>
+    <mergeCell ref="O19:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16296,11 +16296,11 @@
         <v>5</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="72" t="str">
+      <c r="C4" s="52" t="str">
         <f>'week 1'!C4</f>
         <v>Jesse</v>
       </c>
-      <c r="D4" s="72"/>
+      <c r="D4" s="52"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -16308,11 +16308,11 @@
         <v>6</v>
       </c>
       <c r="I4" s="2"/>
-      <c r="J4" s="72" t="str">
+      <c r="J4" s="52" t="str">
         <f>'week 1'!J4</f>
         <v>NHL Stenden</v>
       </c>
-      <c r="K4" s="72"/>
+      <c r="K4" s="52"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -16338,11 +16338,11 @@
         <v>7</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="72" t="str">
+      <c r="C6" s="52" t="str">
         <f>'week 1'!C6</f>
         <v>Hendrik Bijlsma</v>
       </c>
-      <c r="D6" s="72"/>
+      <c r="D6" s="52"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -16350,11 +16350,11 @@
         <v>8</v>
       </c>
       <c r="I6" s="2"/>
-      <c r="J6" s="72" t="str">
+      <c r="J6" s="52" t="str">
         <f>'week 1'!J6</f>
         <v>Cees Naatvlees</v>
       </c>
-      <c r="K6" s="72"/>
+      <c r="K6" s="52"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -16421,18 +16421,18 @@
       <c r="C10" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="73" t="s">
+      <c r="D10" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="73"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="53"/>
+      <c r="M10" s="53"/>
       <c r="N10" s="76"/>
       <c r="O10" s="43" t="s">
         <v>38</v>
@@ -16442,25 +16442,25 @@
       <c r="A11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="71">
+      <c r="B11" s="75">
         <f>C12-C11-O11</f>
         <v>0</v>
       </c>
       <c r="C11" s="25">
         <v>0</v>
       </c>
-      <c r="D11" s="52"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="53"/>
-      <c r="N11" s="54"/>
-      <c r="O11" s="74">
+      <c r="D11" s="56"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="50">
         <v>0</v>
       </c>
     </row>
@@ -16469,46 +16469,46 @@
         <f>F2</f>
         <v>45714</v>
       </c>
-      <c r="B12" s="51"/>
+      <c r="B12" s="55"/>
       <c r="C12" s="26">
         <v>0</v>
       </c>
-      <c r="D12" s="55"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="56"/>
-      <c r="L12" s="56"/>
-      <c r="M12" s="56"/>
-      <c r="N12" s="57"/>
-      <c r="O12" s="75"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="60"/>
+      <c r="N12" s="61"/>
+      <c r="O12" s="51"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="71">
+      <c r="B13" s="75">
         <f>C14-C13-O13</f>
         <v>0</v>
       </c>
       <c r="C13" s="25">
         <v>0</v>
       </c>
-      <c r="D13" s="58"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59"/>
-      <c r="N13" s="60"/>
-      <c r="O13" s="74">
+      <c r="D13" s="62"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="63"/>
+      <c r="L13" s="63"/>
+      <c r="M13" s="63"/>
+      <c r="N13" s="64"/>
+      <c r="O13" s="50">
         <v>0</v>
       </c>
     </row>
@@ -16517,46 +16517,46 @@
         <f>A12+1</f>
         <v>45715</v>
       </c>
-      <c r="B14" s="51"/>
+      <c r="B14" s="55"/>
       <c r="C14" s="26">
         <v>0</v>
       </c>
-      <c r="D14" s="55"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="56"/>
-      <c r="L14" s="56"/>
-      <c r="M14" s="56"/>
-      <c r="N14" s="57"/>
-      <c r="O14" s="75"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="60"/>
+      <c r="N14" s="61"/>
+      <c r="O14" s="51"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="71">
+      <c r="B15" s="75">
         <f>C16-C15-O15</f>
         <v>0</v>
       </c>
       <c r="C15" s="25">
         <v>0</v>
       </c>
-      <c r="D15" s="58"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="59"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="59"/>
-      <c r="N15" s="60"/>
-      <c r="O15" s="74">
+      <c r="D15" s="62"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="63"/>
+      <c r="L15" s="63"/>
+      <c r="M15" s="63"/>
+      <c r="N15" s="64"/>
+      <c r="O15" s="50">
         <v>0</v>
       </c>
     </row>
@@ -16565,45 +16565,45 @@
         <f>A14+1</f>
         <v>45716</v>
       </c>
-      <c r="B16" s="51"/>
+      <c r="B16" s="55"/>
       <c r="C16" s="26">
         <v>0</v>
       </c>
-      <c r="D16" s="55"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="56"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="56"/>
-      <c r="L16" s="56"/>
-      <c r="M16" s="56"/>
-      <c r="N16" s="57"/>
-      <c r="O16" s="75"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="60"/>
+      <c r="L16" s="60"/>
+      <c r="M16" s="60"/>
+      <c r="N16" s="61"/>
+      <c r="O16" s="51"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="71">
+      <c r="B17" s="75">
         <f>C18-C17-O17</f>
         <v>0</v>
       </c>
       <c r="C17" s="25">
         <v>0</v>
       </c>
-      <c r="D17" s="58"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="59"/>
-      <c r="H17" s="59"/>
-      <c r="I17" s="59"/>
-      <c r="J17" s="59"/>
-      <c r="K17" s="59"/>
-      <c r="L17" s="59"/>
-      <c r="M17" s="59"/>
-      <c r="N17" s="60"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="63"/>
+      <c r="L17" s="63"/>
+      <c r="M17" s="63"/>
+      <c r="N17" s="64"/>
       <c r="O17" s="77">
         <v>0</v>
       </c>
@@ -16613,45 +16613,45 @@
         <f>A16+1</f>
         <v>45717</v>
       </c>
-      <c r="B18" s="51"/>
+      <c r="B18" s="55"/>
       <c r="C18" s="26">
         <v>0</v>
       </c>
-      <c r="D18" s="55"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="56"/>
-      <c r="K18" s="56"/>
-      <c r="L18" s="56"/>
-      <c r="M18" s="56"/>
-      <c r="N18" s="57"/>
-      <c r="O18" s="75"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="60"/>
+      <c r="N18" s="61"/>
+      <c r="O18" s="51"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="71">
+      <c r="B19" s="75">
         <f>C20-C19-O19</f>
         <v>0</v>
       </c>
       <c r="C19" s="25">
         <v>0</v>
       </c>
-      <c r="D19" s="58"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="59"/>
-      <c r="H19" s="59"/>
-      <c r="I19" s="59"/>
-      <c r="J19" s="59"/>
-      <c r="K19" s="59"/>
-      <c r="L19" s="59"/>
-      <c r="M19" s="59"/>
-      <c r="N19" s="60"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="63"/>
+      <c r="L19" s="63"/>
+      <c r="M19" s="63"/>
+      <c r="N19" s="64"/>
       <c r="O19" s="77">
         <v>0</v>
       </c>
@@ -16661,22 +16661,22 @@
         <f>A18+1</f>
         <v>45718</v>
       </c>
-      <c r="B20" s="51"/>
+      <c r="B20" s="55"/>
       <c r="C20" s="26">
         <v>0</v>
       </c>
-      <c r="D20" s="55"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="56"/>
-      <c r="K20" s="56"/>
-      <c r="L20" s="56"/>
-      <c r="M20" s="56"/>
-      <c r="N20" s="57"/>
-      <c r="O20" s="75"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="60"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="60"/>
+      <c r="J20" s="60"/>
+      <c r="K20" s="60"/>
+      <c r="L20" s="60"/>
+      <c r="M20" s="60"/>
+      <c r="N20" s="61"/>
+      <c r="O20" s="51"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
@@ -16695,7 +16695,7 @@
       <c r="N21" s="2"/>
     </row>
     <row r="22" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="61" t="s">
+      <c r="A22" s="65" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="14" t="s">
@@ -16717,51 +16717,51 @@
       <c r="N22" s="2"/>
     </row>
     <row r="23" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="62"/>
-      <c r="B23" s="64"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="64"/>
-      <c r="I23" s="65"/>
-      <c r="J23" s="65"/>
-      <c r="K23" s="65"/>
-      <c r="L23" s="65"/>
-      <c r="M23" s="66"/>
+      <c r="A23" s="66"/>
+      <c r="B23" s="68"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="69"/>
+      <c r="J23" s="69"/>
+      <c r="K23" s="69"/>
+      <c r="L23" s="69"/>
+      <c r="M23" s="70"/>
       <c r="N23" s="2"/>
     </row>
     <row r="24" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="62"/>
-      <c r="B24" s="67"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="67"/>
-      <c r="I24" s="65"/>
-      <c r="J24" s="65"/>
-      <c r="K24" s="65"/>
-      <c r="L24" s="65"/>
-      <c r="M24" s="66"/>
+      <c r="A24" s="66"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="69"/>
+      <c r="K24" s="69"/>
+      <c r="L24" s="69"/>
+      <c r="M24" s="70"/>
       <c r="N24" s="2"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="63"/>
-      <c r="B25" s="68"/>
-      <c r="C25" s="69"/>
-      <c r="D25" s="69"/>
-      <c r="E25" s="69"/>
-      <c r="F25" s="69"/>
-      <c r="G25" s="70"/>
-      <c r="H25" s="68"/>
-      <c r="I25" s="69"/>
-      <c r="J25" s="69"/>
-      <c r="K25" s="69"/>
-      <c r="L25" s="69"/>
-      <c r="M25" s="70"/>
+      <c r="A25" s="67"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="73"/>
+      <c r="J25" s="73"/>
+      <c r="K25" s="73"/>
+      <c r="L25" s="73"/>
+      <c r="M25" s="74"/>
       <c r="N25" s="2"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
@@ -16788,7 +16788,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="49">
         <f>SUM(B11:B20,'week 3'!D27)</f>
-        <v>0.20833333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
@@ -16831,16 +16831,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="O17:O18"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="D10:N10"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="D11:N12"/>
     <mergeCell ref="D13:N14"/>
@@ -16854,6 +16844,16 @@
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="D17:N18"/>
     <mergeCell ref="D19:N20"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="D10:N10"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="O17:O18"/>
+    <mergeCell ref="O19:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16946,10 +16946,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="72" t="s">
+      <c r="C4" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="72"/>
+      <c r="D4" s="52"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -16957,10 +16957,10 @@
         <v>6</v>
       </c>
       <c r="I4" s="2"/>
-      <c r="J4" s="72" t="s">
+      <c r="J4" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="K4" s="72"/>
+      <c r="K4" s="52"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -16986,10 +16986,10 @@
         <v>7</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="72" t="s">
+      <c r="C6" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="72"/>
+      <c r="D6" s="52"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -16997,10 +16997,10 @@
         <v>8</v>
       </c>
       <c r="I6" s="2"/>
-      <c r="J6" s="72" t="s">
+      <c r="J6" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="K6" s="72"/>
+      <c r="K6" s="52"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -17067,18 +17067,18 @@
       <c r="C10" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="73" t="s">
+      <c r="D10" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="73"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="53"/>
+      <c r="M10" s="53"/>
       <c r="N10" s="76"/>
       <c r="O10" s="43" t="s">
         <v>38</v>
@@ -17088,23 +17088,23 @@
       <c r="A11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="71">
+      <c r="B11" s="75">
         <f>C12-C11-O11</f>
         <v>0</v>
       </c>
       <c r="C11" s="25"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="53"/>
-      <c r="N11" s="54"/>
-      <c r="O11" s="74">
+      <c r="D11" s="56"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="50">
         <v>0</v>
       </c>
     </row>
@@ -17113,43 +17113,43 @@
         <f>F2</f>
         <v>45721</v>
       </c>
-      <c r="B12" s="51"/>
+      <c r="B12" s="55"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="56"/>
-      <c r="L12" s="56"/>
-      <c r="M12" s="56"/>
-      <c r="N12" s="57"/>
-      <c r="O12" s="75"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="60"/>
+      <c r="N12" s="61"/>
+      <c r="O12" s="51"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="71">
+      <c r="B13" s="75">
         <f>C14-C13-O13</f>
         <v>0</v>
       </c>
       <c r="C13" s="25">
         <v>0</v>
       </c>
-      <c r="D13" s="58"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59"/>
-      <c r="N13" s="60"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="63"/>
+      <c r="L13" s="63"/>
+      <c r="M13" s="63"/>
+      <c r="N13" s="64"/>
       <c r="O13" s="77">
         <v>0</v>
       </c>
@@ -17159,43 +17159,43 @@
         <f>A12+1</f>
         <v>45722</v>
       </c>
-      <c r="B14" s="51"/>
+      <c r="B14" s="55"/>
       <c r="C14" s="26">
         <v>0</v>
       </c>
-      <c r="D14" s="55"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="56"/>
-      <c r="L14" s="56"/>
-      <c r="M14" s="56"/>
-      <c r="N14" s="57"/>
-      <c r="O14" s="75"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="60"/>
+      <c r="N14" s="61"/>
+      <c r="O14" s="51"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="71">
+      <c r="B15" s="75">
         <f>C16-C15-O15</f>
         <v>0</v>
       </c>
       <c r="C15" s="25"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="59"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="59"/>
-      <c r="N15" s="60"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="63"/>
+      <c r="L15" s="63"/>
+      <c r="M15" s="63"/>
+      <c r="N15" s="64"/>
       <c r="O15" s="77">
         <v>0</v>
       </c>
@@ -17205,43 +17205,43 @@
         <f>A14+1</f>
         <v>45723</v>
       </c>
-      <c r="B16" s="51"/>
+      <c r="B16" s="55"/>
       <c r="C16" s="26"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="56"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="56"/>
-      <c r="L16" s="56"/>
-      <c r="M16" s="56"/>
-      <c r="N16" s="57"/>
-      <c r="O16" s="75"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="60"/>
+      <c r="L16" s="60"/>
+      <c r="M16" s="60"/>
+      <c r="N16" s="61"/>
+      <c r="O16" s="51"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="71">
+      <c r="B17" s="75">
         <f>C18-C17-O17</f>
         <v>0</v>
       </c>
       <c r="C17" s="25">
         <v>0</v>
       </c>
-      <c r="D17" s="58"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="59"/>
-      <c r="H17" s="59"/>
-      <c r="I17" s="59"/>
-      <c r="J17" s="59"/>
-      <c r="K17" s="59"/>
-      <c r="L17" s="59"/>
-      <c r="M17" s="59"/>
-      <c r="N17" s="60"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="63"/>
+      <c r="L17" s="63"/>
+      <c r="M17" s="63"/>
+      <c r="N17" s="64"/>
       <c r="O17" s="77">
         <v>0</v>
       </c>
@@ -17251,45 +17251,45 @@
         <f>A16+1</f>
         <v>45724</v>
       </c>
-      <c r="B18" s="51"/>
+      <c r="B18" s="55"/>
       <c r="C18" s="26">
         <v>0</v>
       </c>
-      <c r="D18" s="55"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="56"/>
-      <c r="K18" s="56"/>
-      <c r="L18" s="56"/>
-      <c r="M18" s="56"/>
-      <c r="N18" s="57"/>
-      <c r="O18" s="75"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="60"/>
+      <c r="N18" s="61"/>
+      <c r="O18" s="51"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="71">
+      <c r="B19" s="75">
         <f>C20-C19-O19</f>
         <v>0</v>
       </c>
       <c r="C19" s="25">
         <v>0</v>
       </c>
-      <c r="D19" s="58"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="59"/>
-      <c r="H19" s="59"/>
-      <c r="I19" s="59"/>
-      <c r="J19" s="59"/>
-      <c r="K19" s="59"/>
-      <c r="L19" s="59"/>
-      <c r="M19" s="59"/>
-      <c r="N19" s="60"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="63"/>
+      <c r="L19" s="63"/>
+      <c r="M19" s="63"/>
+      <c r="N19" s="64"/>
       <c r="O19" s="77">
         <v>0</v>
       </c>
@@ -17299,22 +17299,22 @@
         <f>A18+1</f>
         <v>45725</v>
       </c>
-      <c r="B20" s="51"/>
+      <c r="B20" s="55"/>
       <c r="C20" s="26">
         <v>0</v>
       </c>
-      <c r="D20" s="55"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="56"/>
-      <c r="K20" s="56"/>
-      <c r="L20" s="56"/>
-      <c r="M20" s="56"/>
-      <c r="N20" s="57"/>
-      <c r="O20" s="75"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="60"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="60"/>
+      <c r="J20" s="60"/>
+      <c r="K20" s="60"/>
+      <c r="L20" s="60"/>
+      <c r="M20" s="60"/>
+      <c r="N20" s="61"/>
+      <c r="O20" s="51"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
@@ -17333,7 +17333,7 @@
       <c r="N21" s="2"/>
     </row>
     <row r="22" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="61" t="s">
+      <c r="A22" s="65" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="14" t="s">
@@ -17355,51 +17355,51 @@
       <c r="N22" s="2"/>
     </row>
     <row r="23" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="62"/>
-      <c r="B23" s="64"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="64"/>
-      <c r="I23" s="65"/>
-      <c r="J23" s="65"/>
-      <c r="K23" s="65"/>
-      <c r="L23" s="65"/>
-      <c r="M23" s="66"/>
+      <c r="A23" s="66"/>
+      <c r="B23" s="68"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="69"/>
+      <c r="J23" s="69"/>
+      <c r="K23" s="69"/>
+      <c r="L23" s="69"/>
+      <c r="M23" s="70"/>
       <c r="N23" s="2"/>
     </row>
     <row r="24" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="62"/>
-      <c r="B24" s="67"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="67"/>
-      <c r="I24" s="65"/>
-      <c r="J24" s="65"/>
-      <c r="K24" s="65"/>
-      <c r="L24" s="65"/>
-      <c r="M24" s="66"/>
+      <c r="A24" s="66"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="69"/>
+      <c r="K24" s="69"/>
+      <c r="L24" s="69"/>
+      <c r="M24" s="70"/>
       <c r="N24" s="2"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="63"/>
-      <c r="B25" s="68"/>
-      <c r="C25" s="69"/>
-      <c r="D25" s="69"/>
-      <c r="E25" s="69"/>
-      <c r="F25" s="69"/>
-      <c r="G25" s="70"/>
-      <c r="H25" s="68"/>
-      <c r="I25" s="69"/>
-      <c r="J25" s="69"/>
-      <c r="K25" s="69"/>
-      <c r="L25" s="69"/>
-      <c r="M25" s="70"/>
+      <c r="A25" s="67"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="73"/>
+      <c r="J25" s="73"/>
+      <c r="K25" s="73"/>
+      <c r="L25" s="73"/>
+      <c r="M25" s="74"/>
       <c r="N25" s="2"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
@@ -17426,7 +17426,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="49">
         <f>SUM(B11:B20,'week 4'!D27)</f>
-        <v>0.20833333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
@@ -17469,16 +17469,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="O17:O18"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="D10:N10"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="D11:N12"/>
     <mergeCell ref="D13:N14"/>
@@ -17492,6 +17482,16 @@
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="D17:N18"/>
     <mergeCell ref="D19:N20"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="D10:N10"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="O17:O18"/>
+    <mergeCell ref="O19:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -17596,11 +17596,11 @@
         <v>5</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="72" t="str">
+      <c r="C4" s="52" t="str">
         <f>'week 1'!C4</f>
         <v>Jesse</v>
       </c>
-      <c r="D4" s="72"/>
+      <c r="D4" s="52"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -17608,11 +17608,11 @@
         <v>6</v>
       </c>
       <c r="I4" s="2"/>
-      <c r="J4" s="72" t="str">
+      <c r="J4" s="52" t="str">
         <f>'week 1'!J4</f>
         <v>NHL Stenden</v>
       </c>
-      <c r="K4" s="72"/>
+      <c r="K4" s="52"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -17638,11 +17638,11 @@
         <v>7</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="72" t="str">
+      <c r="C6" s="52" t="str">
         <f>'week 1'!C6</f>
         <v>Hendrik Bijlsma</v>
       </c>
-      <c r="D6" s="72"/>
+      <c r="D6" s="52"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -17650,11 +17650,11 @@
         <v>8</v>
       </c>
       <c r="I6" s="2"/>
-      <c r="J6" s="72" t="str">
+      <c r="J6" s="52" t="str">
         <f>'week 1'!J6</f>
         <v>Cees Naatvlees</v>
       </c>
-      <c r="K6" s="72"/>
+      <c r="K6" s="52"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -17721,18 +17721,18 @@
       <c r="C10" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="73" t="s">
+      <c r="D10" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="73"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="53"/>
+      <c r="M10" s="53"/>
       <c r="N10" s="76"/>
       <c r="O10" s="43" t="s">
         <v>38</v>
@@ -17742,25 +17742,25 @@
       <c r="A11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="71">
+      <c r="B11" s="75">
         <f>C12-C11-O11</f>
         <v>0</v>
       </c>
       <c r="C11" s="25">
         <v>0</v>
       </c>
-      <c r="D11" s="52"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="53"/>
-      <c r="N11" s="54"/>
-      <c r="O11" s="74">
+      <c r="D11" s="56"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="50">
         <v>0</v>
       </c>
     </row>
@@ -17769,45 +17769,45 @@
         <f>F2</f>
         <v>45728</v>
       </c>
-      <c r="B12" s="51"/>
+      <c r="B12" s="55"/>
       <c r="C12" s="26">
         <v>0</v>
       </c>
-      <c r="D12" s="55"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="56"/>
-      <c r="L12" s="56"/>
-      <c r="M12" s="56"/>
-      <c r="N12" s="57"/>
-      <c r="O12" s="75"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="60"/>
+      <c r="N12" s="61"/>
+      <c r="O12" s="51"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="71">
+      <c r="B13" s="75">
         <f>C14-C13-O13</f>
         <v>0</v>
       </c>
       <c r="C13" s="25">
         <v>0</v>
       </c>
-      <c r="D13" s="58"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59"/>
-      <c r="N13" s="60"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="63"/>
+      <c r="L13" s="63"/>
+      <c r="M13" s="63"/>
+      <c r="N13" s="64"/>
       <c r="O13" s="77">
         <v>0</v>
       </c>
@@ -17817,45 +17817,45 @@
         <f>A12+1</f>
         <v>45729</v>
       </c>
-      <c r="B14" s="51"/>
+      <c r="B14" s="55"/>
       <c r="C14" s="26">
         <v>0</v>
       </c>
-      <c r="D14" s="55"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="56"/>
-      <c r="L14" s="56"/>
-      <c r="M14" s="56"/>
-      <c r="N14" s="57"/>
-      <c r="O14" s="75"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="60"/>
+      <c r="N14" s="61"/>
+      <c r="O14" s="51"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="71">
+      <c r="B15" s="75">
         <f>C16-C15-O15</f>
         <v>0</v>
       </c>
       <c r="C15" s="25">
         <v>0</v>
       </c>
-      <c r="D15" s="58"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="59"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="59"/>
-      <c r="N15" s="60"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="63"/>
+      <c r="L15" s="63"/>
+      <c r="M15" s="63"/>
+      <c r="N15" s="64"/>
       <c r="O15" s="77">
         <v>0</v>
       </c>
@@ -17865,45 +17865,45 @@
         <f>A14+1</f>
         <v>45730</v>
       </c>
-      <c r="B16" s="51"/>
+      <c r="B16" s="55"/>
       <c r="C16" s="26">
         <v>0</v>
       </c>
-      <c r="D16" s="55"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="56"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="56"/>
-      <c r="L16" s="56"/>
-      <c r="M16" s="56"/>
-      <c r="N16" s="57"/>
-      <c r="O16" s="75"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="60"/>
+      <c r="L16" s="60"/>
+      <c r="M16" s="60"/>
+      <c r="N16" s="61"/>
+      <c r="O16" s="51"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="71">
+      <c r="B17" s="75">
         <f>C18-C17-O17</f>
         <v>0</v>
       </c>
       <c r="C17" s="25">
         <v>0</v>
       </c>
-      <c r="D17" s="58"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="59"/>
-      <c r="H17" s="59"/>
-      <c r="I17" s="59"/>
-      <c r="J17" s="59"/>
-      <c r="K17" s="59"/>
-      <c r="L17" s="59"/>
-      <c r="M17" s="59"/>
-      <c r="N17" s="60"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="63"/>
+      <c r="L17" s="63"/>
+      <c r="M17" s="63"/>
+      <c r="N17" s="64"/>
       <c r="O17" s="77">
         <v>0</v>
       </c>
@@ -17913,45 +17913,45 @@
         <f>A16+1</f>
         <v>45731</v>
       </c>
-      <c r="B18" s="51"/>
+      <c r="B18" s="55"/>
       <c r="C18" s="26">
         <v>0</v>
       </c>
-      <c r="D18" s="55"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="56"/>
-      <c r="K18" s="56"/>
-      <c r="L18" s="56"/>
-      <c r="M18" s="56"/>
-      <c r="N18" s="57"/>
-      <c r="O18" s="75"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="60"/>
+      <c r="N18" s="61"/>
+      <c r="O18" s="51"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="71">
+      <c r="B19" s="75">
         <f>C20-C19-O19</f>
         <v>0</v>
       </c>
       <c r="C19" s="25">
         <v>0</v>
       </c>
-      <c r="D19" s="58"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="59"/>
-      <c r="H19" s="59"/>
-      <c r="I19" s="59"/>
-      <c r="J19" s="59"/>
-      <c r="K19" s="59"/>
-      <c r="L19" s="59"/>
-      <c r="M19" s="59"/>
-      <c r="N19" s="60"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="63"/>
+      <c r="L19" s="63"/>
+      <c r="M19" s="63"/>
+      <c r="N19" s="64"/>
       <c r="O19" s="77">
         <v>0</v>
       </c>
@@ -17961,22 +17961,22 @@
         <f>A18+1</f>
         <v>45732</v>
       </c>
-      <c r="B20" s="51"/>
+      <c r="B20" s="55"/>
       <c r="C20" s="26">
         <v>0</v>
       </c>
-      <c r="D20" s="55"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="56"/>
-      <c r="K20" s="56"/>
-      <c r="L20" s="56"/>
-      <c r="M20" s="56"/>
-      <c r="N20" s="57"/>
-      <c r="O20" s="75"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="60"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="60"/>
+      <c r="J20" s="60"/>
+      <c r="K20" s="60"/>
+      <c r="L20" s="60"/>
+      <c r="M20" s="60"/>
+      <c r="N20" s="61"/>
+      <c r="O20" s="51"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
@@ -17995,7 +17995,7 @@
       <c r="N21" s="2"/>
     </row>
     <row r="22" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="61" t="s">
+      <c r="A22" s="65" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="14" t="s">
@@ -18017,51 +18017,51 @@
       <c r="N22" s="2"/>
     </row>
     <row r="23" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="62"/>
-      <c r="B23" s="64"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="64"/>
-      <c r="I23" s="65"/>
-      <c r="J23" s="65"/>
-      <c r="K23" s="65"/>
-      <c r="L23" s="65"/>
-      <c r="M23" s="66"/>
+      <c r="A23" s="66"/>
+      <c r="B23" s="68"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="69"/>
+      <c r="J23" s="69"/>
+      <c r="K23" s="69"/>
+      <c r="L23" s="69"/>
+      <c r="M23" s="70"/>
       <c r="N23" s="2"/>
     </row>
     <row r="24" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="62"/>
-      <c r="B24" s="67"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="67"/>
-      <c r="I24" s="65"/>
-      <c r="J24" s="65"/>
-      <c r="K24" s="65"/>
-      <c r="L24" s="65"/>
-      <c r="M24" s="66"/>
+      <c r="A24" s="66"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="69"/>
+      <c r="K24" s="69"/>
+      <c r="L24" s="69"/>
+      <c r="M24" s="70"/>
       <c r="N24" s="2"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="63"/>
-      <c r="B25" s="68"/>
-      <c r="C25" s="69"/>
-      <c r="D25" s="69"/>
-      <c r="E25" s="69"/>
-      <c r="F25" s="69"/>
-      <c r="G25" s="70"/>
-      <c r="H25" s="68"/>
-      <c r="I25" s="69"/>
-      <c r="J25" s="69"/>
-      <c r="K25" s="69"/>
-      <c r="L25" s="69"/>
-      <c r="M25" s="70"/>
+      <c r="A25" s="67"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="73"/>
+      <c r="J25" s="73"/>
+      <c r="K25" s="73"/>
+      <c r="L25" s="73"/>
+      <c r="M25" s="74"/>
       <c r="N25" s="2"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
@@ -18088,7 +18088,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="49">
         <f>SUM(B11:B20,'week 5'!D27)</f>
-        <v>0.20833333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
@@ -18131,16 +18131,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="O17:O18"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="D10:N10"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="D11:N12"/>
     <mergeCell ref="D13:N14"/>
@@ -18154,6 +18144,16 @@
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="D17:N18"/>
     <mergeCell ref="D19:N20"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="D10:N10"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="O17:O18"/>
+    <mergeCell ref="O19:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18246,11 +18246,11 @@
         <v>5</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="72" t="str">
+      <c r="C4" s="52" t="str">
         <f>'week 1'!C4</f>
         <v>Jesse</v>
       </c>
-      <c r="D4" s="72"/>
+      <c r="D4" s="52"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -18258,11 +18258,11 @@
         <v>6</v>
       </c>
       <c r="I4" s="2"/>
-      <c r="J4" s="72" t="str">
+      <c r="J4" s="52" t="str">
         <f>'week 1'!J4</f>
         <v>NHL Stenden</v>
       </c>
-      <c r="K4" s="72"/>
+      <c r="K4" s="52"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -18288,11 +18288,11 @@
         <v>7</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="72" t="str">
+      <c r="C6" s="52" t="str">
         <f>'week 1'!C6</f>
         <v>Hendrik Bijlsma</v>
       </c>
-      <c r="D6" s="72"/>
+      <c r="D6" s="52"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -18300,11 +18300,11 @@
         <v>8</v>
       </c>
       <c r="I6" s="2"/>
-      <c r="J6" s="72" t="str">
+      <c r="J6" s="52" t="str">
         <f>'week 1'!J6</f>
         <v>Cees Naatvlees</v>
       </c>
-      <c r="K6" s="72"/>
+      <c r="K6" s="52"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -18371,18 +18371,18 @@
       <c r="C10" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="73" t="s">
+      <c r="D10" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="73"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="53"/>
+      <c r="M10" s="53"/>
       <c r="N10" s="76"/>
       <c r="O10" s="43" t="s">
         <v>38</v>
@@ -18392,25 +18392,25 @@
       <c r="A11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="71">
+      <c r="B11" s="75">
         <f>C12-C11-O11</f>
         <v>0</v>
       </c>
       <c r="C11" s="25">
         <v>0</v>
       </c>
-      <c r="D11" s="52"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="53"/>
-      <c r="N11" s="54"/>
-      <c r="O11" s="74">
+      <c r="D11" s="56"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="50">
         <v>0</v>
       </c>
     </row>
@@ -18419,45 +18419,45 @@
         <f>F2</f>
         <v>45735</v>
       </c>
-      <c r="B12" s="51"/>
+      <c r="B12" s="55"/>
       <c r="C12" s="26">
         <v>0</v>
       </c>
-      <c r="D12" s="55"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="56"/>
-      <c r="L12" s="56"/>
-      <c r="M12" s="56"/>
-      <c r="N12" s="57"/>
-      <c r="O12" s="75"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="60"/>
+      <c r="N12" s="61"/>
+      <c r="O12" s="51"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="71">
+      <c r="B13" s="75">
         <f>C14-C13-O13</f>
         <v>0</v>
       </c>
       <c r="C13" s="25">
         <v>0</v>
       </c>
-      <c r="D13" s="58"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59"/>
-      <c r="N13" s="60"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="63"/>
+      <c r="L13" s="63"/>
+      <c r="M13" s="63"/>
+      <c r="N13" s="64"/>
       <c r="O13" s="77">
         <v>0</v>
       </c>
@@ -18467,45 +18467,45 @@
         <f>A12+1</f>
         <v>45736</v>
       </c>
-      <c r="B14" s="51"/>
+      <c r="B14" s="55"/>
       <c r="C14" s="26">
         <v>0</v>
       </c>
-      <c r="D14" s="55"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="56"/>
-      <c r="L14" s="56"/>
-      <c r="M14" s="56"/>
-      <c r="N14" s="57"/>
-      <c r="O14" s="75"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="60"/>
+      <c r="N14" s="61"/>
+      <c r="O14" s="51"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="71">
+      <c r="B15" s="75">
         <f>C16-C15-O15</f>
         <v>0</v>
       </c>
       <c r="C15" s="25">
         <v>0</v>
       </c>
-      <c r="D15" s="58"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="59"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="59"/>
-      <c r="N15" s="60"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="63"/>
+      <c r="L15" s="63"/>
+      <c r="M15" s="63"/>
+      <c r="N15" s="64"/>
       <c r="O15" s="77">
         <v>0</v>
       </c>
@@ -18515,45 +18515,45 @@
         <f>A14+1</f>
         <v>45737</v>
       </c>
-      <c r="B16" s="51"/>
+      <c r="B16" s="55"/>
       <c r="C16" s="26">
         <v>0</v>
       </c>
-      <c r="D16" s="55"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="56"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="56"/>
-      <c r="L16" s="56"/>
-      <c r="M16" s="56"/>
-      <c r="N16" s="57"/>
-      <c r="O16" s="75"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="60"/>
+      <c r="L16" s="60"/>
+      <c r="M16" s="60"/>
+      <c r="N16" s="61"/>
+      <c r="O16" s="51"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="71">
+      <c r="B17" s="75">
         <f>C18-C17-O17</f>
         <v>0</v>
       </c>
       <c r="C17" s="25">
         <v>0</v>
       </c>
-      <c r="D17" s="58"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="59"/>
-      <c r="H17" s="59"/>
-      <c r="I17" s="59"/>
-      <c r="J17" s="59"/>
-      <c r="K17" s="59"/>
-      <c r="L17" s="59"/>
-      <c r="M17" s="59"/>
-      <c r="N17" s="60"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="63"/>
+      <c r="L17" s="63"/>
+      <c r="M17" s="63"/>
+      <c r="N17" s="64"/>
       <c r="O17" s="77">
         <v>0</v>
       </c>
@@ -18563,45 +18563,45 @@
         <f>A16+1</f>
         <v>45738</v>
       </c>
-      <c r="B18" s="51"/>
+      <c r="B18" s="55"/>
       <c r="C18" s="26">
         <v>0</v>
       </c>
-      <c r="D18" s="55"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="56"/>
-      <c r="K18" s="56"/>
-      <c r="L18" s="56"/>
-      <c r="M18" s="56"/>
-      <c r="N18" s="57"/>
-      <c r="O18" s="75"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="60"/>
+      <c r="N18" s="61"/>
+      <c r="O18" s="51"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="71">
+      <c r="B19" s="75">
         <f>C20-C19-O19</f>
         <v>0</v>
       </c>
       <c r="C19" s="25">
         <v>0</v>
       </c>
-      <c r="D19" s="58"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="59"/>
-      <c r="H19" s="59"/>
-      <c r="I19" s="59"/>
-      <c r="J19" s="59"/>
-      <c r="K19" s="59"/>
-      <c r="L19" s="59"/>
-      <c r="M19" s="59"/>
-      <c r="N19" s="60"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="63"/>
+      <c r="L19" s="63"/>
+      <c r="M19" s="63"/>
+      <c r="N19" s="64"/>
       <c r="O19" s="77">
         <v>0</v>
       </c>
@@ -18611,22 +18611,22 @@
         <f>A18+1</f>
         <v>45739</v>
       </c>
-      <c r="B20" s="51"/>
+      <c r="B20" s="55"/>
       <c r="C20" s="26">
         <v>0</v>
       </c>
-      <c r="D20" s="55"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="56"/>
-      <c r="K20" s="56"/>
-      <c r="L20" s="56"/>
-      <c r="M20" s="56"/>
-      <c r="N20" s="57"/>
-      <c r="O20" s="75"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="60"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="60"/>
+      <c r="J20" s="60"/>
+      <c r="K20" s="60"/>
+      <c r="L20" s="60"/>
+      <c r="M20" s="60"/>
+      <c r="N20" s="61"/>
+      <c r="O20" s="51"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
@@ -18645,7 +18645,7 @@
       <c r="N21" s="2"/>
     </row>
     <row r="22" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="61" t="s">
+      <c r="A22" s="65" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="14" t="s">
@@ -18667,51 +18667,51 @@
       <c r="N22" s="2"/>
     </row>
     <row r="23" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="62"/>
-      <c r="B23" s="64"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="64"/>
-      <c r="I23" s="65"/>
-      <c r="J23" s="65"/>
-      <c r="K23" s="65"/>
-      <c r="L23" s="65"/>
-      <c r="M23" s="66"/>
+      <c r="A23" s="66"/>
+      <c r="B23" s="68"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="69"/>
+      <c r="J23" s="69"/>
+      <c r="K23" s="69"/>
+      <c r="L23" s="69"/>
+      <c r="M23" s="70"/>
       <c r="N23" s="2"/>
     </row>
     <row r="24" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="62"/>
-      <c r="B24" s="67"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="67"/>
-      <c r="I24" s="65"/>
-      <c r="J24" s="65"/>
-      <c r="K24" s="65"/>
-      <c r="L24" s="65"/>
-      <c r="M24" s="66"/>
+      <c r="A24" s="66"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="69"/>
+      <c r="K24" s="69"/>
+      <c r="L24" s="69"/>
+      <c r="M24" s="70"/>
       <c r="N24" s="2"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="63"/>
-      <c r="B25" s="68"/>
-      <c r="C25" s="69"/>
-      <c r="D25" s="69"/>
-      <c r="E25" s="69"/>
-      <c r="F25" s="69"/>
-      <c r="G25" s="70"/>
-      <c r="H25" s="68"/>
-      <c r="I25" s="69"/>
-      <c r="J25" s="69"/>
-      <c r="K25" s="69"/>
-      <c r="L25" s="69"/>
-      <c r="M25" s="70"/>
+      <c r="A25" s="67"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="73"/>
+      <c r="J25" s="73"/>
+      <c r="K25" s="73"/>
+      <c r="L25" s="73"/>
+      <c r="M25" s="74"/>
       <c r="N25" s="2"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
@@ -18738,7 +18738,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="49">
         <f>SUM(B11:B20,'week 6'!D27)</f>
-        <v>0.20833333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
@@ -18781,16 +18781,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="O17:O18"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="D10:N10"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="D11:N12"/>
     <mergeCell ref="D13:N14"/>
@@ -18804,6 +18794,16 @@
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="D17:N18"/>
     <mergeCell ref="D19:N20"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="D10:N10"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="O17:O18"/>
+    <mergeCell ref="O19:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -18908,11 +18908,11 @@
         <v>5</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="72" t="str">
+      <c r="C4" s="52" t="str">
         <f>'week 1'!C4</f>
         <v>Jesse</v>
       </c>
-      <c r="D4" s="72"/>
+      <c r="D4" s="52"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -18920,11 +18920,11 @@
         <v>6</v>
       </c>
       <c r="I4" s="2"/>
-      <c r="J4" s="72" t="str">
+      <c r="J4" s="52" t="str">
         <f>'week 1'!J4</f>
         <v>NHL Stenden</v>
       </c>
-      <c r="K4" s="72"/>
+      <c r="K4" s="52"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -18950,11 +18950,11 @@
         <v>7</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="72" t="str">
+      <c r="C6" s="52" t="str">
         <f>'week 1'!C6</f>
         <v>Hendrik Bijlsma</v>
       </c>
-      <c r="D6" s="72"/>
+      <c r="D6" s="52"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -18962,11 +18962,11 @@
         <v>8</v>
       </c>
       <c r="I6" s="2"/>
-      <c r="J6" s="72" t="str">
+      <c r="J6" s="52" t="str">
         <f>'week 1'!J6</f>
         <v>Cees Naatvlees</v>
       </c>
-      <c r="K6" s="72"/>
+      <c r="K6" s="52"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -19033,18 +19033,18 @@
       <c r="C10" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="73" t="s">
+      <c r="D10" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="73"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="53"/>
+      <c r="M10" s="53"/>
       <c r="N10" s="76"/>
       <c r="O10" s="43" t="s">
         <v>38</v>
@@ -19054,25 +19054,25 @@
       <c r="A11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="71">
+      <c r="B11" s="75">
         <f>C12-C11-O11</f>
         <v>0</v>
       </c>
       <c r="C11" s="25">
         <v>0</v>
       </c>
-      <c r="D11" s="52"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="53"/>
-      <c r="N11" s="54"/>
-      <c r="O11" s="74">
+      <c r="D11" s="56"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="50">
         <v>0</v>
       </c>
     </row>
@@ -19081,45 +19081,45 @@
         <f>F2</f>
         <v>45742</v>
       </c>
-      <c r="B12" s="51"/>
+      <c r="B12" s="55"/>
       <c r="C12" s="26">
         <v>0</v>
       </c>
-      <c r="D12" s="55"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="56"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="56"/>
-      <c r="L12" s="56"/>
-      <c r="M12" s="56"/>
-      <c r="N12" s="57"/>
-      <c r="O12" s="75"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="60"/>
+      <c r="N12" s="61"/>
+      <c r="O12" s="51"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="71">
+      <c r="B13" s="75">
         <f>C14-C13-O13</f>
         <v>0</v>
       </c>
       <c r="C13" s="25">
         <v>0</v>
       </c>
-      <c r="D13" s="58"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59"/>
-      <c r="N13" s="60"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="63"/>
+      <c r="L13" s="63"/>
+      <c r="M13" s="63"/>
+      <c r="N13" s="64"/>
       <c r="O13" s="77">
         <v>0</v>
       </c>
@@ -19129,45 +19129,45 @@
         <f>A12+1</f>
         <v>45743</v>
       </c>
-      <c r="B14" s="51"/>
+      <c r="B14" s="55"/>
       <c r="C14" s="26">
         <v>0</v>
       </c>
-      <c r="D14" s="55"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="56"/>
-      <c r="L14" s="56"/>
-      <c r="M14" s="56"/>
-      <c r="N14" s="57"/>
-      <c r="O14" s="75"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="60"/>
+      <c r="N14" s="61"/>
+      <c r="O14" s="51"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="71">
+      <c r="B15" s="75">
         <f>C16-C15-O15</f>
         <v>0</v>
       </c>
       <c r="C15" s="25">
         <v>0</v>
       </c>
-      <c r="D15" s="58"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="59"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="59"/>
-      <c r="N15" s="60"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="63"/>
+      <c r="L15" s="63"/>
+      <c r="M15" s="63"/>
+      <c r="N15" s="64"/>
       <c r="O15" s="77">
         <v>0</v>
       </c>
@@ -19177,45 +19177,45 @@
         <f>A14+1</f>
         <v>45744</v>
       </c>
-      <c r="B16" s="51"/>
+      <c r="B16" s="55"/>
       <c r="C16" s="26">
         <v>0</v>
       </c>
-      <c r="D16" s="55"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="56"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="56"/>
-      <c r="L16" s="56"/>
-      <c r="M16" s="56"/>
-      <c r="N16" s="57"/>
-      <c r="O16" s="75"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="60"/>
+      <c r="L16" s="60"/>
+      <c r="M16" s="60"/>
+      <c r="N16" s="61"/>
+      <c r="O16" s="51"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="71">
+      <c r="B17" s="75">
         <f>C18-C17-O17</f>
         <v>0</v>
       </c>
       <c r="C17" s="25">
         <v>0</v>
       </c>
-      <c r="D17" s="58"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="59"/>
-      <c r="H17" s="59"/>
-      <c r="I17" s="59"/>
-      <c r="J17" s="59"/>
-      <c r="K17" s="59"/>
-      <c r="L17" s="59"/>
-      <c r="M17" s="59"/>
-      <c r="N17" s="60"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="63"/>
+      <c r="L17" s="63"/>
+      <c r="M17" s="63"/>
+      <c r="N17" s="64"/>
       <c r="O17" s="77">
         <v>0</v>
       </c>
@@ -19225,45 +19225,45 @@
         <f>A16+1</f>
         <v>45745</v>
       </c>
-      <c r="B18" s="51"/>
+      <c r="B18" s="55"/>
       <c r="C18" s="26">
         <v>0</v>
       </c>
-      <c r="D18" s="55"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="56"/>
-      <c r="K18" s="56"/>
-      <c r="L18" s="56"/>
-      <c r="M18" s="56"/>
-      <c r="N18" s="57"/>
-      <c r="O18" s="75"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="60"/>
+      <c r="N18" s="61"/>
+      <c r="O18" s="51"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="71">
+      <c r="B19" s="75">
         <f>C20-C19-O19</f>
         <v>0</v>
       </c>
       <c r="C19" s="25">
         <v>0</v>
       </c>
-      <c r="D19" s="58"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="59"/>
-      <c r="H19" s="59"/>
-      <c r="I19" s="59"/>
-      <c r="J19" s="59"/>
-      <c r="K19" s="59"/>
-      <c r="L19" s="59"/>
-      <c r="M19" s="59"/>
-      <c r="N19" s="60"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="63"/>
+      <c r="L19" s="63"/>
+      <c r="M19" s="63"/>
+      <c r="N19" s="64"/>
       <c r="O19" s="77">
         <v>0</v>
       </c>
@@ -19273,22 +19273,22 @@
         <f>A18+1</f>
         <v>45746</v>
       </c>
-      <c r="B20" s="51"/>
+      <c r="B20" s="55"/>
       <c r="C20" s="26">
         <v>0</v>
       </c>
-      <c r="D20" s="55"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="56"/>
-      <c r="K20" s="56"/>
-      <c r="L20" s="56"/>
-      <c r="M20" s="56"/>
-      <c r="N20" s="57"/>
-      <c r="O20" s="75"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="60"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="60"/>
+      <c r="J20" s="60"/>
+      <c r="K20" s="60"/>
+      <c r="L20" s="60"/>
+      <c r="M20" s="60"/>
+      <c r="N20" s="61"/>
+      <c r="O20" s="51"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
@@ -19307,7 +19307,7 @@
       <c r="N21" s="2"/>
     </row>
     <row r="22" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="61" t="s">
+      <c r="A22" s="65" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="14" t="s">
@@ -19329,51 +19329,51 @@
       <c r="N22" s="2"/>
     </row>
     <row r="23" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="62"/>
-      <c r="B23" s="64"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="64"/>
-      <c r="I23" s="65"/>
-      <c r="J23" s="65"/>
-      <c r="K23" s="65"/>
-      <c r="L23" s="65"/>
-      <c r="M23" s="66"/>
+      <c r="A23" s="66"/>
+      <c r="B23" s="68"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="69"/>
+      <c r="J23" s="69"/>
+      <c r="K23" s="69"/>
+      <c r="L23" s="69"/>
+      <c r="M23" s="70"/>
       <c r="N23" s="2"/>
     </row>
     <row r="24" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="62"/>
-      <c r="B24" s="67"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="67"/>
-      <c r="I24" s="65"/>
-      <c r="J24" s="65"/>
-      <c r="K24" s="65"/>
-      <c r="L24" s="65"/>
-      <c r="M24" s="66"/>
+      <c r="A24" s="66"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="69"/>
+      <c r="K24" s="69"/>
+      <c r="L24" s="69"/>
+      <c r="M24" s="70"/>
       <c r="N24" s="2"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="63"/>
-      <c r="B25" s="68"/>
-      <c r="C25" s="69"/>
-      <c r="D25" s="69"/>
-      <c r="E25" s="69"/>
-      <c r="F25" s="69"/>
-      <c r="G25" s="70"/>
-      <c r="H25" s="68"/>
-      <c r="I25" s="69"/>
-      <c r="J25" s="69"/>
-      <c r="K25" s="69"/>
-      <c r="L25" s="69"/>
-      <c r="M25" s="70"/>
+      <c r="A25" s="67"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="73"/>
+      <c r="J25" s="73"/>
+      <c r="K25" s="73"/>
+      <c r="L25" s="73"/>
+      <c r="M25" s="74"/>
       <c r="N25" s="2"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
@@ -19400,7 +19400,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="49">
         <f>SUM(B11:B20,'week 7'!D27)</f>
-        <v>0.20833333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
@@ -19443,16 +19443,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="O17:O18"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="D10:N10"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="D13:N14"/>
     <mergeCell ref="D11:N12"/>
@@ -19466,6 +19456,16 @@
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="D17:N18"/>
     <mergeCell ref="D19:N20"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="D10:N10"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="O17:O18"/>
+    <mergeCell ref="O19:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -19862,7 +19862,7 @@
       </c>
       <c r="C7" s="38">
         <f>'week 1'!B17</f>
-        <v>6.2499999999999944E-2</v>
+        <v>0.10416666666666663</v>
       </c>
       <c r="D7" s="36"/>
       <c r="E7" s="44" t="s">
@@ -20044,7 +20044,7 @@
     <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24" s="48">
         <f>'week 1'!D28</f>
-        <v>0.20833333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="B24" s="48">
         <f>'week 2'!D28</f>
@@ -20090,7 +20090,7 @@
       </c>
       <c r="R24" s="36">
         <f>SUM(C7,G7,K7,O7,S7,W7,AA7,AE7)</f>
-        <v>6.2499999999999944E-2</v>
+        <v>0.10416666666666663</v>
       </c>
       <c r="S24" s="36">
         <f>SUM(C8,G8,K8,O8,S8,W8,AA8,AE8)</f>
@@ -20190,6 +20190,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2311421a-1a78-47dc-a354-ac7cd3350930">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c229a3ec-9035-4016-afff-d65ac05ad1ff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100620D60D3A7791A408192F9577A622611" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="6d60ec7fb257b476c7e22b24fdeb809b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2311421a-1a78-47dc-a354-ac7cd3350930" xmlns:ns3="c229a3ec-9035-4016-afff-d65ac05ad1ff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="60329889ea8ef2a5b5bc5aca08810b53" ns2:_="" ns3:_="">
     <xsd:import namespace="2311421a-1a78-47dc-a354-ac7cd3350930"/>
@@ -20392,27 +20412,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED771D81-13A9-4225-8AFE-4E2129F69B97}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2311421a-1a78-47dc-a354-ac7cd3350930"/>
+    <ds:schemaRef ds:uri="c229a3ec-9035-4016-afff-d65ac05ad1ff"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2311421a-1a78-47dc-a354-ac7cd3350930">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="c229a3ec-9035-4016-afff-d65ac05ad1ff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95246B6B-5867-475C-A1FA-BAC082A87CBF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{852518A3-07B4-4E61-9724-DAD571943AC8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20429,23 +20448,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95246B6B-5867-475C-A1FA-BAC082A87CBF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED771D81-13A9-4225-8AFE-4E2129F69B97}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2311421a-1a78-47dc-a354-ac7cd3350930"/>
-    <ds:schemaRef ds:uri="c229a3ec-9035-4016-afff-d65ac05ad1ff"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
uren aangepast en document
</commit_message>
<xml_diff>
--- a/Documentatie/Urenverantwoording/Jesse/urenverantwoording sjabloom Jesse Ernste.xlsx
+++ b/Documentatie/Urenverantwoording/Jesse/urenverantwoording sjabloom Jesse Ernste.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesse\Documents\GitHub\Project-digitale-besturing\Documentatie\Urenverantwoording\Jesse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C0813E-9F00-49E7-AFBF-78FDC84EE307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58FAAFFF-5766-4EA9-9C41-32564415DC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="50">
   <si>
     <t>Urenverantwoordingsformulier</t>
   </si>
@@ -180,6 +180,18 @@
   </si>
   <si>
     <t>Vergadering , plannen en taken verdelen.</t>
+  </si>
+  <si>
+    <t>documentatiewerkzaamheden, inventerisatie programmeren</t>
+  </si>
+  <si>
+    <t>Cees Draaier</t>
+  </si>
+  <si>
+    <t>Plan van aanpak formuleren</t>
+  </si>
+  <si>
+    <t>uitleg project</t>
   </si>
 </sst>
 </file>
@@ -1170,7 +1182,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>6.25E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.14583333333333337</c:v>
@@ -1394,7 +1406,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>6.25E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.14583333333333337</c:v>
@@ -1759,7 +1771,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>6.25E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.14583333333333337</c:v>
@@ -2126,7 +2138,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>6.25E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.14583333333333337</c:v>
@@ -2808,10 +2820,10 @@
                 <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.3125</c:v>
+                  <c:v>0.375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.16666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -3186,10 +3198,10 @@
                 <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.10416666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.14583333333333337</c:v>
@@ -3554,10 +3566,10 @@
                 <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.10416666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>6.25E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -6987,7 +6999,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>6.25E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.14583333333333337</c:v>
@@ -6999,10 +7011,10 @@
                   <c:v>6.25E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.10416666666666663</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>6.25E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -14057,8 +14069,8 @@
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19:O20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14190,7 +14202,7 @@
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="72" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="K6" s="72"/>
       <c r="L6" s="2"/>
@@ -14334,12 +14346,14 @@
       </c>
       <c r="B13" s="71">
         <f>C14-C13-O13</f>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="C13" s="27">
-        <v>0</v>
-      </c>
-      <c r="D13" s="58"/>
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D13" s="58" t="s">
+        <v>49</v>
+      </c>
       <c r="E13" s="59"/>
       <c r="F13" s="59"/>
       <c r="G13" s="59"/>
@@ -14363,7 +14377,7 @@
       </c>
       <c r="B14" s="51"/>
       <c r="C14" s="26">
-        <v>0</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D14" s="55"/>
       <c r="E14" s="56"/>
@@ -14642,7 +14656,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="49">
         <f>B11+B13+B15+B17+B19</f>
-        <v>0.3125</v>
+        <v>0.375</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
@@ -14665,7 +14679,7 @@
       <c r="C28" s="2"/>
       <c r="D28" s="49">
         <f>SUM(B11:B20)</f>
-        <v>0.3125</v>
+        <v>0.375</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2" t="s">
@@ -14915,8 +14929,8 @@
   <sheetPr codeName="Blad2"/>
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15053,7 +15067,7 @@
       <c r="I6" s="2"/>
       <c r="J6" s="72" t="str">
         <f>'week 1'!J6</f>
-        <v>Cees Naatvlees</v>
+        <v>Cees Draaier</v>
       </c>
       <c r="K6" s="72"/>
       <c r="L6" s="2"/>
@@ -15145,12 +15159,14 @@
       </c>
       <c r="B11" s="71">
         <f>C12-C11-O11</f>
-        <v>0</v>
+        <v>0.10416666666666663</v>
       </c>
       <c r="C11" s="27">
-        <v>0</v>
-      </c>
-      <c r="D11" s="52"/>
+        <v>0.4375</v>
+      </c>
+      <c r="D11" s="52" t="s">
+        <v>46</v>
+      </c>
       <c r="E11" s="53"/>
       <c r="F11" s="53"/>
       <c r="G11" s="53"/>
@@ -15172,7 +15188,7 @@
       </c>
       <c r="B12" s="51"/>
       <c r="C12" s="26">
-        <v>0</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="D12" s="55"/>
       <c r="E12" s="56"/>
@@ -15193,12 +15209,14 @@
       </c>
       <c r="B13" s="71">
         <f>C14-C13-O13</f>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="C13" s="27">
-        <v>0</v>
-      </c>
-      <c r="D13" s="58"/>
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="D13" s="58" t="s">
+        <v>48</v>
+      </c>
       <c r="E13" s="59"/>
       <c r="F13" s="59"/>
       <c r="G13" s="59"/>
@@ -15220,7 +15238,7 @@
       </c>
       <c r="B14" s="51"/>
       <c r="C14" s="26">
-        <v>0</v>
+        <v>0.44791666666666669</v>
       </c>
       <c r="D14" s="55"/>
       <c r="E14" s="56"/>
@@ -15489,7 +15507,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="49">
         <f>SUM(B11:B20,'week 1'!D27)</f>
-        <v>0.3125</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
@@ -15512,7 +15530,7 @@
       <c r="C28" s="2"/>
       <c r="D28" s="49">
         <f>SUM(B11:B20)</f>
-        <v>0</v>
+        <v>0.16666666666666663</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2" t="s">
@@ -15705,7 +15723,7 @@
       <c r="I6" s="2"/>
       <c r="J6" s="72" t="str">
         <f>'week 1'!J6</f>
-        <v>Cees Naatvlees</v>
+        <v>Cees Draaier</v>
       </c>
       <c r="K6" s="72"/>
       <c r="L6" s="2"/>
@@ -16141,7 +16159,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="49">
         <f>SUM(B11:B20,'week 2'!D27)</f>
-        <v>0.3125</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
@@ -16218,7 +16236,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16354,7 +16372,7 @@
       <c r="I6" s="2"/>
       <c r="J6" s="72" t="str">
         <f>'week 1'!J6</f>
-        <v>Cees Naatvlees</v>
+        <v>Cees Draaier</v>
       </c>
       <c r="K6" s="72"/>
       <c r="L6" s="2"/>
@@ -16790,7 +16808,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="49">
         <f>SUM(B11:B20,'week 3'!D27)</f>
-        <v>0.3125</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
@@ -16867,7 +16885,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17:O18"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17428,7 +17446,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="49">
         <f>SUM(B11:B20,'week 4'!D27)</f>
-        <v>0.3125</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
@@ -17654,7 +17672,7 @@
       <c r="I6" s="2"/>
       <c r="J6" s="72" t="str">
         <f>'week 1'!J6</f>
-        <v>Cees Naatvlees</v>
+        <v>Cees Draaier</v>
       </c>
       <c r="K6" s="72"/>
       <c r="L6" s="2"/>
@@ -18090,7 +18108,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="49">
         <f>SUM(B11:B20,'week 5'!D27)</f>
-        <v>0.3125</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
@@ -18304,7 +18322,7 @@
       <c r="I6" s="2"/>
       <c r="J6" s="72" t="str">
         <f>'week 1'!J6</f>
-        <v>Cees Naatvlees</v>
+        <v>Cees Draaier</v>
       </c>
       <c r="K6" s="72"/>
       <c r="L6" s="2"/>
@@ -18740,7 +18758,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="49">
         <f>SUM(B11:B20,'week 6'!D27)</f>
-        <v>0.3125</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
@@ -18966,7 +18984,7 @@
       <c r="I6" s="2"/>
       <c r="J6" s="72" t="str">
         <f>'week 1'!J6</f>
-        <v>Cees Naatvlees</v>
+        <v>Cees Draaier</v>
       </c>
       <c r="K6" s="72"/>
       <c r="L6" s="2"/>
@@ -19402,7 +19420,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="49">
         <f>SUM(B11:B20,'week 7'!D27)</f>
-        <v>0.3125</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
@@ -19600,7 +19618,7 @@
       </c>
       <c r="G4" s="45">
         <f>'week 2'!B11</f>
-        <v>0</v>
+        <v>0.10416666666666663</v>
       </c>
       <c r="H4" s="36"/>
       <c r="I4" s="44" t="s">
@@ -19680,7 +19698,7 @@
       </c>
       <c r="C5" s="38">
         <f>'week 1'!B13</f>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="D5" s="36"/>
       <c r="E5" s="44" t="s">
@@ -19692,7 +19710,7 @@
       </c>
       <c r="G5" s="45">
         <f>'week 2'!B13</f>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="H5" s="36"/>
       <c r="I5" s="44" t="s">
@@ -20046,11 +20064,11 @@
     <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24" s="48">
         <f>'week 1'!D28</f>
-        <v>0.3125</v>
+        <v>0.375</v>
       </c>
       <c r="B24" s="48">
         <f>'week 2'!D28</f>
-        <v>0</v>
+        <v>0.16666666666666663</v>
       </c>
       <c r="C24" s="48">
         <f>'week 3'!D28</f>
@@ -20080,11 +20098,11 @@
       <c r="M24" s="36"/>
       <c r="O24" s="36">
         <f>SUM(C4,G4,K4,O4,S4,W4,AA4,AE4)</f>
-        <v>0</v>
+        <v>0.10416666666666663</v>
       </c>
       <c r="P24" s="36">
         <f>SUM(C5,G5,K5,O5,S5,W5,AA5,AE5)</f>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="Q24" s="36">
         <f>SUM(C6,G6,K6,O6,S6,W6,AA6,AE6)</f>

</xml_diff>